<commit_message>
Inicio do documento de product backlog
</commit_message>
<xml_diff>
--- a/Documentação/planilha requisitos.xlsx
+++ b/Documentação/planilha requisitos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ultim\Desktop\BandTec\git\novoProjeto\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ultim\Desktop\BandTec\git\boxzard\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB07D77F-08A1-4A61-A8EF-0C15A7DB0781}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D3FEB3-062E-4887-A0A2-95DC9A82730C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548" xr2:uid="{62812CE9-B7D2-4317-BEDF-1A63102B2E36}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{62812CE9-B7D2-4317-BEDF-1A63102B2E36}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha de Requisitos" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="80">
   <si>
     <t>id</t>
   </si>
@@ -200,9 +200,6 @@
     <t>Notificações</t>
   </si>
   <si>
-    <t>Enviar notificações sobre a temperatura e umidade em que seus produtos estão sendo mantidos.</t>
-  </si>
-  <si>
     <t>Gerar relatório sobre as informações desejadas sobre o serviço contratado e os dados que o envolvem.</t>
   </si>
   <si>
@@ -258,6 +255,21 @@
   </si>
   <si>
     <t>RF018</t>
+  </si>
+  <si>
+    <t>RF0010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tabelas banco de dados </t>
+  </si>
+  <si>
+    <t>produto, temperatura ideal e umidade e usuario, temperatura ambiente</t>
+  </si>
+  <si>
+    <t>Essencial</t>
+  </si>
+  <si>
+    <t>Enviar notificações sobre a temperatura e umidade em que seus produtos estão sendo mantidos. (email)</t>
   </si>
 </sst>
 </file>
@@ -305,7 +317,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -515,11 +527,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -534,13 +588,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -615,15 +663,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -662,6 +701,45 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -976,27 +1054,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1AC4D2-7026-4F35-A980-9AD1E4D216BB}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="25.21875" customWidth="1"/>
-    <col min="4" max="4" width="51.21875" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1006,340 +1084,364 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="16" t="s">
+      <c r="B3" s="50"/>
+      <c r="C3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="50"/>
+      <c r="C4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="18" t="s">
         <v>7</v>
       </c>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="16" t="s">
+      <c r="B5" s="50"/>
+      <c r="C5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="16" t="s">
+      <c r="B6" s="50"/>
+      <c r="C6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="23" t="s">
+      <c r="B7" s="50"/>
+      <c r="C7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="27" t="s">
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="12" t="s">
+      <c r="B8" s="50"/>
+      <c r="C8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="12" t="s">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="50"/>
+      <c r="C9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+      <c r="E9" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="51"/>
+      <c r="C10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="53" t="s">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="56"/>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="47" t="s">
+      <c r="B13" s="50"/>
+      <c r="C13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="33" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="39" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="38" t="s">
+      <c r="B14" s="50"/>
+      <c r="C14" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="50"/>
+      <c r="C15" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="50"/>
+      <c r="C16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="50"/>
+      <c r="C17" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="51"/>
+      <c r="C18" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="43" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="41" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="44" t="s">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="42" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="43" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="48" t="s">
+      <c r="C19" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="42" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="28" t="s">
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="54"/>
+      <c r="C20" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="60"/>
+      <c r="C21" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="59" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="53"/>
+      <c r="C22" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="47" t="s">
+      <c r="E22" s="45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E19" s="38" t="s">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="31" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="52" t="s">
+    <row r="24" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="E20" s="50" t="s">
+      <c r="B24" s="53"/>
+      <c r="C24" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="31" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A3:A20">
+  <sortState ref="A3:A22">
     <sortCondition ref="A2"/>
   </sortState>
   <mergeCells count="4">
     <mergeCell ref="B2:B10"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="B19:B22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização modelo conceitual 1.0
</commit_message>
<xml_diff>
--- a/Documentação/planilha requisitos.xlsx
+++ b/Documentação/planilha requisitos.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ultim\Desktop\BandTec\git\boxzard\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF79BED-9609-401F-ADCC-6B18E2E5E56D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105006AD-2901-42E5-83BE-3C52DC526885}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="2" xr2:uid="{62812CE9-B7D2-4317-BEDF-1A63102B2E36}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548" activeTab="2" xr2:uid="{62812CE9-B7D2-4317-BEDF-1A63102B2E36}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
     <sheet name="Planilha de Requisitos" sheetId="1" r:id="rId2"/>
-    <sheet name="Sprint Backlog" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint Backlog (29-03)" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Planilha de Requisitos'!$A$1:$E$7</definedName>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="177">
   <si>
     <t>id</t>
   </si>
@@ -337,9 +337,6 @@
     <t>Ler dados vindos do sensor dht11.</t>
   </si>
   <si>
-    <t>Comparar Temperatura</t>
-  </si>
-  <si>
     <t>Compara a temperatura e umidade lida dos sensores com a do banco.</t>
   </si>
   <si>
@@ -566,6 +563,9 @@
   </si>
   <si>
     <t>Criação de tabelas</t>
+  </si>
+  <si>
+    <t>Modelo Conceitual</t>
   </si>
 </sst>
 </file>
@@ -663,7 +663,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -687,17 +687,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1036,37 +1025,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1078,64 +1041,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1148,64 +1093,88 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1526,14 +1495,14 @@
       <selection activeCell="A21" sqref="A21:E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -1550,11 +1519,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="24">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="53" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="14" t="s">
@@ -1567,11 +1536,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="54"/>
       <c r="C3" s="5" t="s">
         <v>53</v>
       </c>
@@ -1582,11 +1551,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="54"/>
       <c r="C4" s="5" t="s">
         <v>54</v>
       </c>
@@ -1597,11 +1566,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="28"/>
+      <c r="B5" s="54"/>
       <c r="C5" s="5" t="s">
         <v>57</v>
       </c>
@@ -1612,11 +1581,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="28"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="5" t="s">
         <v>59</v>
       </c>
@@ -1627,11 +1596,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>6</v>
       </c>
-      <c r="B7" s="28"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="6" t="s">
         <v>61</v>
       </c>
@@ -1642,11 +1611,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>7</v>
       </c>
-      <c r="B8" s="28"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="5" t="s">
         <v>63</v>
       </c>
@@ -1657,11 +1626,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="20">
         <v>8</v>
       </c>
-      <c r="B9" s="29"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="21" t="s">
         <v>65</v>
       </c>
@@ -1672,14 +1641,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
       <c r="D10" s="4"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -1696,11 +1665,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>9</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="53" t="s">
         <v>67</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -1713,11 +1682,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <v>10</v>
       </c>
-      <c r="B13" s="28"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="5" t="s">
         <v>70</v>
       </c>
@@ -1728,11 +1697,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>11</v>
       </c>
-      <c r="B14" s="28"/>
+      <c r="B14" s="54"/>
       <c r="C14" s="5" t="s">
         <v>72</v>
       </c>
@@ -1743,11 +1712,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>12</v>
       </c>
-      <c r="B15" s="28"/>
+      <c r="B15" s="54"/>
       <c r="C15" s="5" t="s">
         <v>74</v>
       </c>
@@ -1758,11 +1727,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>13</v>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="5" t="s">
         <v>80</v>
       </c>
@@ -1773,11 +1742,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>14</v>
       </c>
-      <c r="B17" s="28"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="6" t="s">
         <v>76</v>
       </c>
@@ -1788,11 +1757,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>15</v>
       </c>
-      <c r="B18" s="28"/>
+      <c r="B18" s="54"/>
       <c r="C18" s="5" t="s">
         <v>95</v>
       </c>
@@ -1803,11 +1772,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="20">
         <v>16</v>
       </c>
-      <c r="B19" s="29"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="21" t="s">
         <v>78</v>
       </c>
@@ -1818,8 +1787,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
@@ -1836,11 +1805,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>17</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="53" t="s">
         <v>82</v>
       </c>
       <c r="C22" s="14" t="s">
@@ -1853,11 +1822,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="17">
         <v>18</v>
       </c>
-      <c r="B23" s="28"/>
+      <c r="B23" s="54"/>
       <c r="C23" s="5" t="s">
         <v>85</v>
       </c>
@@ -1868,11 +1837,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>19</v>
       </c>
-      <c r="B24" s="28"/>
+      <c r="B24" s="54"/>
       <c r="C24" s="5" t="s">
         <v>87</v>
       </c>
@@ -1883,11 +1852,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>20</v>
       </c>
-      <c r="B25" s="28"/>
+      <c r="B25" s="54"/>
       <c r="C25" s="5" t="s">
         <v>89</v>
       </c>
@@ -1898,11 +1867,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>21</v>
       </c>
-      <c r="B26" s="28"/>
+      <c r="B26" s="54"/>
       <c r="C26" s="5" t="s">
         <v>91</v>
       </c>
@@ -1913,11 +1882,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>22</v>
       </c>
-      <c r="B27" s="28"/>
+      <c r="B27" s="54"/>
       <c r="C27" s="6" t="s">
         <v>93</v>
       </c>
@@ -1943,56 +1912,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1AC4D2-7026-4F35-A980-9AD1E4D216BB}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C5" sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="44" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="27" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="31"/>
+      <c r="B3" s="57"/>
       <c r="C3" s="5" t="s">
         <v>85</v>
       </c>
@@ -2004,11 +1973,11 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="31"/>
+      <c r="B4" s="57"/>
       <c r="C4" s="5" t="s">
         <v>87</v>
       </c>
@@ -2020,26 +1989,26 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="31"/>
+      <c r="B5" s="57"/>
       <c r="C5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>100</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>101</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="31"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="5" t="s">
         <v>91</v>
       </c>
@@ -2050,12 +2019,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="34" t="s">
+      <c r="B7" s="58"/>
+      <c r="C7" s="28" t="s">
         <v>85</v>
       </c>
       <c r="D7" s="22" t="s">
@@ -2065,140 +2034,140 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="35"/>
-    </row>
-    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="29"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="29"/>
+    </row>
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>102</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>103</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="42" t="s">
+      <c r="B10" s="57"/>
+      <c r="C10" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="37" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="31"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>104</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>105</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="B12" s="31"/>
+        <v>152</v>
+      </c>
+      <c r="B12" s="57"/>
       <c r="C12" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>106</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>107</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="B13" s="31"/>
+        <v>153</v>
+      </c>
+      <c r="B13" s="57"/>
       <c r="C13" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>108</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>109</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="31"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>111</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="31"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>112</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>113</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="31"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="31"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="6" t="s">
         <v>57</v>
       </c>
@@ -2209,266 +2178,266 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="31"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>115</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>116</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="31"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>117</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>118</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="31"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>119</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>120</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="B21" s="31"/>
+        <v>154</v>
+      </c>
+      <c r="B21" s="57"/>
       <c r="C21" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>121</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>122</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="B22" s="31"/>
+        <v>155</v>
+      </c>
+      <c r="B22" s="57"/>
       <c r="C22" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>123</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>124</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="B23" s="31"/>
+        <v>156</v>
+      </c>
+      <c r="B23" s="57"/>
       <c r="C23" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>125</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>126</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="B24" s="31"/>
+        <v>157</v>
+      </c>
+      <c r="B24" s="57"/>
       <c r="C24" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="12" t="s">
         <v>127</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>128</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="B25" s="31"/>
+        <v>158</v>
+      </c>
+      <c r="B25" s="57"/>
       <c r="C25" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>129</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>130</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="B26" s="31"/>
+        <v>159</v>
+      </c>
+      <c r="B26" s="57"/>
       <c r="C26" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D26" s="12" t="s">
         <v>131</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>132</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="B27" s="31"/>
+        <v>160</v>
+      </c>
+      <c r="B27" s="57"/>
       <c r="C27" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D27" s="12" t="s">
         <v>149</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>150</v>
       </c>
       <c r="E27" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="B28" s="31"/>
+        <v>161</v>
+      </c>
+      <c r="B28" s="57"/>
       <c r="C28" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D28" s="12" t="s">
         <v>151</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>152</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="B29" s="31"/>
+        <v>162</v>
+      </c>
+      <c r="B29" s="57"/>
       <c r="C29" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E29" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="B30" s="31"/>
+        <v>163</v>
+      </c>
+      <c r="B30" s="57"/>
       <c r="C30" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>134</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>135</v>
       </c>
       <c r="E30" s="18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" s="57"/>
+      <c r="C31" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31" s="37" t="s">
         <v>136</v>
-      </c>
-      <c r="D31" s="43" t="s">
-        <v>137</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="B32" s="31"/>
+        <v>165</v>
+      </c>
+      <c r="B32" s="57"/>
       <c r="C32" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="B33" s="31"/>
+        <v>166</v>
+      </c>
+      <c r="B33" s="57"/>
       <c r="C33" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D33" s="12" t="s">
         <v>142</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>143</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="B34" s="31"/>
+        <v>167</v>
+      </c>
+      <c r="B34" s="57"/>
       <c r="C34" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D34" s="12" t="s">
         <v>144</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>145</v>
       </c>
       <c r="E34" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="B35" s="31"/>
+        <v>168</v>
+      </c>
+      <c r="B35" s="57"/>
       <c r="C35" s="5" t="s">
         <v>31</v>
       </c>
@@ -2479,11 +2448,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="B36" s="31"/>
+        <v>169</v>
+      </c>
+      <c r="B36" s="57"/>
       <c r="C36" s="6" t="s">
         <v>33</v>
       </c>
@@ -2494,33 +2463,33 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="B37" s="33"/>
-      <c r="C37" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="B37" s="58"/>
+      <c r="C37" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="D37" s="22" t="s">
         <v>140</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>141</v>
       </c>
       <c r="E37" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="35"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="35"/>
-    </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="29"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="29"/>
+    </row>
+    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="30" t="s">
+      <c r="B39" s="56" t="s">
         <v>40</v>
       </c>
       <c r="C39" s="14" t="s">
@@ -2533,11 +2502,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="31"/>
+      <c r="B40" s="57"/>
       <c r="C40" s="5" t="s">
         <v>27</v>
       </c>
@@ -2548,13 +2517,13 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="33"/>
+      <c r="B41" s="58"/>
       <c r="C41" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>42</v>
@@ -2563,35 +2532,35 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="35"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="35"/>
-    </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="29"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="29"/>
+    </row>
+    <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C43" s="45" t="s">
+      <c r="C43" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="D43" s="15" t="s">
         <v>147</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>148</v>
       </c>
       <c r="E43" s="16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="31"/>
+      <c r="B44" s="57"/>
       <c r="C44" s="5" t="s">
         <v>17</v>
       </c>
@@ -2602,12 +2571,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="B45" s="33"/>
-      <c r="C45" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="B45" s="58"/>
+      <c r="C45" s="28" t="s">
         <v>25</v>
       </c>
       <c r="D45" s="22" t="s">
@@ -2635,114 +2604,144 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB8FA7D-215A-423D-A0CE-12EFD18E3EEC}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="71" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="72" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="67">
+        <v>1</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="69" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="46"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="48">
+        <v>2</v>
+      </c>
+      <c r="B3" s="59"/>
+      <c r="C3" s="45" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="54" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="54" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="55" t="s">
+      <c r="D3" s="49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="48">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="57">
-        <v>1</v>
-      </c>
-      <c r="B2" s="58" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="48">
+        <v>4</v>
+      </c>
+      <c r="B5" s="59"/>
+      <c r="C5" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="48">
+        <v>5</v>
+      </c>
+      <c r="B6" s="59"/>
+      <c r="C6" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="50">
         <v>6</v>
       </c>
-      <c r="C2" s="59" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="60" t="s">
+      <c r="B7" s="60"/>
+      <c r="C7" s="51" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="52"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="61">
-        <v>2</v>
-      </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="51" t="s">
-        <v>174</v>
-      </c>
-      <c r="D3" s="62" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="47">
+        <v>8</v>
+      </c>
+      <c r="B8" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="64" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" s="65" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="61">
-        <v>3</v>
-      </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="62" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="61">
-        <v>4</v>
-      </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="62" t="s">
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="50">
+        <v>7</v>
+      </c>
+      <c r="B9" s="66"/>
+      <c r="C9" s="51" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" s="52" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="63">
-        <v>5</v>
-      </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="65" t="s">
-        <v>175</v>
-      </c>
-      <c r="D6" s="66" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="67">
-        <v>6</v>
-      </c>
-      <c r="B7" s="68" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="69" t="s">
-        <v>176</v>
-      </c>
-      <c r="D7" s="70" t="s">
-        <v>47</v>
-      </c>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:B6"/>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização documentação - Modelo conceitual, Planilha e Contexto de negocio
</commit_message>
<xml_diff>
--- a/Documentação/planilha requisitos.xlsx
+++ b/Documentação/planilha requisitos.xlsx
@@ -8,17 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ultim\Desktop\BandTec\git\boxzard\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105006AD-2901-42E5-83BE-3C52DC526885}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9B3665-B6F1-4630-8EC2-BAC73C1B2FC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548" activeTab="2" xr2:uid="{62812CE9-B7D2-4317-BEDF-1A63102B2E36}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{62812CE9-B7D2-4317-BEDF-1A63102B2E36}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
     <sheet name="Planilha de Requisitos" sheetId="1" r:id="rId2"/>
-    <sheet name="Sprint Backlog (29-03)" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint BandTec (2°)" sheetId="5" r:id="rId3"/>
+    <sheet name="Sprint Backlog (29-03)" sheetId="3" r:id="rId4"/>
+    <sheet name="Sprint Backlog (05-04)" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Planilha de Requisitos'!$A$1:$E$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sprint BandTec (2°)'!$A$1:$D$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="205">
   <si>
     <t>id</t>
   </si>
@@ -566,13 +569,97 @@
   </si>
   <si>
     <t>Modelo Conceitual</t>
+  </si>
+  <si>
+    <t>Testar banco de dados</t>
+  </si>
+  <si>
+    <t>Banco de dados inserido no Azure</t>
+  </si>
+  <si>
+    <t>Cadastro</t>
+  </si>
+  <si>
+    <t>Arquitetura</t>
+  </si>
+  <si>
+    <t>HLD</t>
+  </si>
+  <si>
+    <t>LLD</t>
+  </si>
+  <si>
+    <t>Prof. Fernando</t>
+  </si>
+  <si>
+    <t>Projetos atualizado no GitHub / Documentação do Projeto Atualizada</t>
+  </si>
+  <si>
+    <t>Planilha de Riscos do Projeto</t>
+  </si>
+  <si>
+    <t>Prof. Yoshi</t>
+  </si>
+  <si>
+    <t>Site Estático Institucional -Local</t>
+  </si>
+  <si>
+    <t>Site Estático Dashboard (Google Charts) -Local</t>
+  </si>
+  <si>
+    <t>Site Estático Cadastro e Login -Local</t>
+  </si>
+  <si>
+    <t>Prof. Alex</t>
+  </si>
+  <si>
+    <t>Ferramenta de Gestão de Projeto Funcionando</t>
+  </si>
+  <si>
+    <t>HLD do Projeto / LLD do Projeto</t>
+  </si>
+  <si>
+    <t>Planilha de BackLog/ Planilha de Sprints</t>
+  </si>
+  <si>
+    <t>Prof. Célia</t>
+  </si>
+  <si>
+    <t>Modelagem Conceitual do Projeto v1</t>
+  </si>
+  <si>
+    <t>Script de criação do Banco / Tabelas criadas no Azure</t>
+  </si>
+  <si>
+    <t>Prof. Marise</t>
+  </si>
+  <si>
+    <t>Teste Integrado (Arduino+DB) + Node.JS Local</t>
+  </si>
+  <si>
+    <t>Diagrama de Arquitetura Local (Arduíno)</t>
+  </si>
+  <si>
+    <t>Especificação do analytics</t>
+  </si>
+  <si>
+    <t>Situação</t>
+  </si>
+  <si>
+    <t>A fazer</t>
+  </si>
+  <si>
+    <t>Em progresso</t>
+  </si>
+  <si>
+    <t>Concluido</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -588,8 +675,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -662,8 +755,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1025,11 +1130,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1129,52 +1260,96 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1491,18 +1666,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809286DD-D5C9-4F7B-AD94-6A53F56382A7}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -1519,11 +1694,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="24">
         <v>1</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="62" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="14" t="s">
@@ -1536,11 +1711,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="54"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="5" t="s">
         <v>53</v>
       </c>
@@ -1551,11 +1726,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="54"/>
+      <c r="B4" s="63"/>
       <c r="C4" s="5" t="s">
         <v>54</v>
       </c>
@@ -1566,11 +1741,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="54"/>
+      <c r="B5" s="63"/>
       <c r="C5" s="5" t="s">
         <v>57</v>
       </c>
@@ -1581,11 +1756,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="54"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="5" t="s">
         <v>59</v>
       </c>
@@ -1596,11 +1771,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>6</v>
       </c>
-      <c r="B7" s="54"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="6" t="s">
         <v>61</v>
       </c>
@@ -1611,11 +1786,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>7</v>
       </c>
-      <c r="B8" s="54"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="5" t="s">
         <v>63</v>
       </c>
@@ -1626,11 +1801,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20">
         <v>8</v>
       </c>
-      <c r="B9" s="55"/>
+      <c r="B9" s="64"/>
       <c r="C9" s="21" t="s">
         <v>65</v>
       </c>
@@ -1641,14 +1816,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
       <c r="D10" s="4"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -1665,11 +1840,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>9</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="62" t="s">
         <v>67</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -1682,11 +1857,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>10</v>
       </c>
-      <c r="B13" s="54"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="5" t="s">
         <v>70</v>
       </c>
@@ -1697,11 +1872,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>11</v>
       </c>
-      <c r="B14" s="54"/>
+      <c r="B14" s="63"/>
       <c r="C14" s="5" t="s">
         <v>72</v>
       </c>
@@ -1712,11 +1887,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>12</v>
       </c>
-      <c r="B15" s="54"/>
+      <c r="B15" s="63"/>
       <c r="C15" s="5" t="s">
         <v>74</v>
       </c>
@@ -1727,11 +1902,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>13</v>
       </c>
-      <c r="B16" s="54"/>
+      <c r="B16" s="63"/>
       <c r="C16" s="5" t="s">
         <v>80</v>
       </c>
@@ -1742,11 +1917,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>14</v>
       </c>
-      <c r="B17" s="54"/>
+      <c r="B17" s="63"/>
       <c r="C17" s="6" t="s">
         <v>76</v>
       </c>
@@ -1757,11 +1932,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>15</v>
       </c>
-      <c r="B18" s="54"/>
+      <c r="B18" s="63"/>
       <c r="C18" s="5" t="s">
         <v>95</v>
       </c>
@@ -1772,11 +1947,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20">
         <v>16</v>
       </c>
-      <c r="B19" s="55"/>
+      <c r="B19" s="64"/>
       <c r="C19" s="21" t="s">
         <v>78</v>
       </c>
@@ -1787,8 +1962,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
@@ -1805,11 +1980,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>17</v>
       </c>
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="62" t="s">
         <v>82</v>
       </c>
       <c r="C22" s="14" t="s">
@@ -1822,11 +1997,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>18</v>
       </c>
-      <c r="B23" s="54"/>
+      <c r="B23" s="63"/>
       <c r="C23" s="5" t="s">
         <v>85</v>
       </c>
@@ -1837,11 +2012,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>19</v>
       </c>
-      <c r="B24" s="54"/>
+      <c r="B24" s="63"/>
       <c r="C24" s="5" t="s">
         <v>87</v>
       </c>
@@ -1852,11 +2027,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>20</v>
       </c>
-      <c r="B25" s="54"/>
+      <c r="B25" s="63"/>
       <c r="C25" s="5" t="s">
         <v>89</v>
       </c>
@@ -1867,11 +2042,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>21</v>
       </c>
-      <c r="B26" s="54"/>
+      <c r="B26" s="63"/>
       <c r="C26" s="5" t="s">
         <v>91</v>
       </c>
@@ -1882,11 +2057,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>22</v>
       </c>
-      <c r="B27" s="54"/>
+      <c r="B27" s="63"/>
       <c r="C27" s="6" t="s">
         <v>93</v>
       </c>
@@ -1912,18 +2087,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1AC4D2-7026-4F35-A980-9AD1E4D216BB}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:E7"/>
+    <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
@@ -1940,11 +2115,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="66" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="34" t="s">
@@ -1957,11 +2132,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="57"/>
+      <c r="B3" s="66"/>
       <c r="C3" s="5" t="s">
         <v>85</v>
       </c>
@@ -1973,11 +2148,11 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="57"/>
+      <c r="B4" s="66"/>
       <c r="C4" s="5" t="s">
         <v>87</v>
       </c>
@@ -1989,11 +2164,11 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="57"/>
+      <c r="B5" s="66"/>
       <c r="C5" s="5" t="s">
         <v>91</v>
       </c>
@@ -2004,11 +2179,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="57"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="5" t="s">
         <v>91</v>
       </c>
@@ -2019,11 +2194,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="58"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="28" t="s">
         <v>85</v>
       </c>
@@ -2034,18 +2209,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29"/>
       <c r="B8" s="30"/>
       <c r="C8" s="31"/>
       <c r="D8" s="32"/>
       <c r="E8" s="29"/>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="65" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="33" t="s">
@@ -2058,11 +2233,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="57"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="36" t="s">
         <v>29</v>
       </c>
@@ -2073,11 +2248,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="57"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="5" t="s">
         <v>103</v>
       </c>
@@ -2088,11 +2263,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="57"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="5" t="s">
         <v>105</v>
       </c>
@@ -2103,11 +2278,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="B13" s="57"/>
+      <c r="B13" s="66"/>
       <c r="C13" s="5" t="s">
         <v>107</v>
       </c>
@@ -2118,11 +2293,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="57"/>
+      <c r="B14" s="66"/>
       <c r="C14" s="5" t="s">
         <v>109</v>
       </c>
@@ -2133,11 +2308,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="57"/>
+      <c r="B15" s="66"/>
       <c r="C15" s="6" t="s">
         <v>111</v>
       </c>
@@ -2148,11 +2323,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="57"/>
+      <c r="B16" s="66"/>
       <c r="C16" s="6" t="s">
         <v>59</v>
       </c>
@@ -2163,11 +2338,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="57"/>
+      <c r="B17" s="66"/>
       <c r="C17" s="6" t="s">
         <v>57</v>
       </c>
@@ -2178,11 +2353,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="57"/>
+      <c r="B18" s="66"/>
       <c r="C18" s="6" t="s">
         <v>114</v>
       </c>
@@ -2193,11 +2368,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="57"/>
+      <c r="B19" s="66"/>
       <c r="C19" s="6" t="s">
         <v>116</v>
       </c>
@@ -2208,11 +2383,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="57"/>
+      <c r="B20" s="66"/>
       <c r="C20" s="6" t="s">
         <v>118</v>
       </c>
@@ -2223,11 +2398,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="B21" s="57"/>
+      <c r="B21" s="66"/>
       <c r="C21" s="6" t="s">
         <v>120</v>
       </c>
@@ -2238,11 +2413,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="B22" s="57"/>
+      <c r="B22" s="66"/>
       <c r="C22" s="6" t="s">
         <v>122</v>
       </c>
@@ -2253,11 +2428,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="B23" s="57"/>
+      <c r="B23" s="66"/>
       <c r="C23" s="6" t="s">
         <v>124</v>
       </c>
@@ -2268,11 +2443,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="B24" s="57"/>
+      <c r="B24" s="66"/>
       <c r="C24" s="6" t="s">
         <v>126</v>
       </c>
@@ -2283,11 +2458,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="B25" s="57"/>
+      <c r="B25" s="66"/>
       <c r="C25" s="6" t="s">
         <v>128</v>
       </c>
@@ -2298,11 +2473,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="B26" s="57"/>
+      <c r="B26" s="66"/>
       <c r="C26" s="6" t="s">
         <v>130</v>
       </c>
@@ -2313,11 +2488,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="B27" s="57"/>
+      <c r="B27" s="66"/>
       <c r="C27" s="6" t="s">
         <v>148</v>
       </c>
@@ -2328,11 +2503,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="B28" s="57"/>
+      <c r="B28" s="66"/>
       <c r="C28" s="6" t="s">
         <v>150</v>
       </c>
@@ -2343,11 +2518,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="B29" s="57"/>
+      <c r="B29" s="66"/>
       <c r="C29" s="6" t="s">
         <v>63</v>
       </c>
@@ -2358,11 +2533,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="B30" s="57"/>
+      <c r="B30" s="66"/>
       <c r="C30" s="6" t="s">
         <v>133</v>
       </c>
@@ -2373,11 +2548,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="B31" s="57"/>
+      <c r="B31" s="66"/>
       <c r="C31" s="36" t="s">
         <v>135</v>
       </c>
@@ -2388,11 +2563,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="B32" s="57"/>
+      <c r="B32" s="66"/>
       <c r="C32" s="5" t="s">
         <v>137</v>
       </c>
@@ -2403,11 +2578,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="B33" s="57"/>
+      <c r="B33" s="66"/>
       <c r="C33" s="5" t="s">
         <v>141</v>
       </c>
@@ -2418,11 +2593,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="B34" s="57"/>
+      <c r="B34" s="66"/>
       <c r="C34" s="5" t="s">
         <v>143</v>
       </c>
@@ -2433,11 +2608,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="B35" s="57"/>
+      <c r="B35" s="66"/>
       <c r="C35" s="5" t="s">
         <v>31</v>
       </c>
@@ -2448,11 +2623,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="B36" s="57"/>
+      <c r="B36" s="66"/>
       <c r="C36" s="6" t="s">
         <v>33</v>
       </c>
@@ -2463,11 +2638,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="B37" s="58"/>
+      <c r="B37" s="67"/>
       <c r="C37" s="28" t="s">
         <v>139</v>
       </c>
@@ -2478,18 +2653,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="29"/>
       <c r="B38" s="30"/>
       <c r="C38" s="31"/>
       <c r="D38" s="32"/>
       <c r="E38" s="29"/>
     </row>
-    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="56" t="s">
+      <c r="B39" s="65" t="s">
         <v>40</v>
       </c>
       <c r="C39" s="14" t="s">
@@ -2502,11 +2677,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="57"/>
+      <c r="B40" s="66"/>
       <c r="C40" s="5" t="s">
         <v>27</v>
       </c>
@@ -2517,11 +2692,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="58"/>
+      <c r="B41" s="67"/>
       <c r="C41" s="21" t="s">
         <v>145</v>
       </c>
@@ -2532,18 +2707,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="29"/>
       <c r="B42" s="30"/>
       <c r="C42" s="38"/>
       <c r="D42" s="32"/>
       <c r="E42" s="29"/>
     </row>
-    <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="56" t="s">
+      <c r="B43" s="65" t="s">
         <v>16</v>
       </c>
       <c r="C43" s="39" t="s">
@@ -2556,11 +2731,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="57"/>
+      <c r="B44" s="66"/>
       <c r="C44" s="5" t="s">
         <v>17</v>
       </c>
@@ -2571,11 +2746,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B45" s="58"/>
+      <c r="B45" s="67"/>
       <c r="C45" s="28" t="s">
         <v>25</v>
       </c>
@@ -2603,54 +2778,263 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368B4F2A-840E-43DD-A714-BED4E8CCE39E}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="74" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="75" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="87" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="47">
+        <v>1</v>
+      </c>
+      <c r="B2" s="86" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" s="88" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="90" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="50">
+        <v>2</v>
+      </c>
+      <c r="B3" s="70"/>
+      <c r="C3" s="89" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" s="93" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="A4" s="47">
+        <v>3</v>
+      </c>
+      <c r="B4" s="86" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="88" t="s">
+        <v>187</v>
+      </c>
+      <c r="D4" s="96" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="A5" s="48">
+        <v>4</v>
+      </c>
+      <c r="B5" s="69"/>
+      <c r="C5" s="85" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" s="94" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="50">
+        <v>5</v>
+      </c>
+      <c r="B6" s="70"/>
+      <c r="C6" s="89" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" s="97" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="A7" s="47">
+        <v>6</v>
+      </c>
+      <c r="B7" s="86" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="88" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="91" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="A8" s="48">
+        <v>7</v>
+      </c>
+      <c r="B8" s="69"/>
+      <c r="C8" s="85" t="s">
+        <v>192</v>
+      </c>
+      <c r="D8" s="98" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="50">
+        <v>8</v>
+      </c>
+      <c r="B9" s="70"/>
+      <c r="C9" s="89" t="s">
+        <v>193</v>
+      </c>
+      <c r="D9" s="92" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="A10" s="47">
+        <v>9</v>
+      </c>
+      <c r="B10" s="86" t="s">
+        <v>194</v>
+      </c>
+      <c r="C10" s="88" t="s">
+        <v>195</v>
+      </c>
+      <c r="D10" s="91" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="50">
+        <v>10</v>
+      </c>
+      <c r="B11" s="70"/>
+      <c r="C11" s="89" t="s">
+        <v>196</v>
+      </c>
+      <c r="D11" s="97" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="47">
+        <v>11</v>
+      </c>
+      <c r="B12" s="86" t="s">
+        <v>197</v>
+      </c>
+      <c r="C12" s="88" t="s">
+        <v>198</v>
+      </c>
+      <c r="D12" s="95" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+      <c r="A13" s="48">
+        <v>12</v>
+      </c>
+      <c r="B13" s="69"/>
+      <c r="C13" s="85" t="s">
+        <v>199</v>
+      </c>
+      <c r="D13" s="94" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="50">
+        <v>13</v>
+      </c>
+      <c r="B14" s="70"/>
+      <c r="C14" s="89" t="s">
+        <v>200</v>
+      </c>
+      <c r="D14" s="93" t="s">
+        <v>202</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D14" xr:uid="{161861C5-1A09-434C-804D-30DFA2AAE944}"/>
+  <mergeCells count="5">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B14"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB8FA7D-215A-423D-A0CE-12EFD18E3EEC}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="59" t="s">
         <v>172</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="61" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="67">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="57">
         <v>1</v>
       </c>
       <c r="B2" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="58" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="46"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="48">
         <v>2</v>
       </c>
-      <c r="B3" s="59"/>
+      <c r="B3" s="69"/>
       <c r="C3" s="45" t="s">
         <v>173</v>
       </c>
@@ -2658,11 +3042,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="48">
         <v>3</v>
       </c>
-      <c r="B4" s="59"/>
+      <c r="B4" s="69"/>
       <c r="C4" s="45" t="s">
         <v>53</v>
       </c>
@@ -2670,11 +3054,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="48">
         <v>4</v>
       </c>
-      <c r="B5" s="59"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="45" t="s">
         <v>57</v>
       </c>
@@ -2682,11 +3066,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="48">
         <v>5</v>
       </c>
-      <c r="B6" s="59"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="45" t="s">
         <v>54</v>
       </c>
@@ -2694,11 +3078,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="50">
         <v>6</v>
       </c>
-      <c r="B7" s="60"/>
+      <c r="B7" s="70"/>
       <c r="C7" s="51" t="s">
         <v>174</v>
       </c>
@@ -2706,25 +3090,25 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="47">
         <v>8</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="55" t="s">
         <v>175</v>
       </c>
-      <c r="D8" s="65" t="s">
+      <c r="D8" s="56" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="50">
         <v>7</v>
       </c>
-      <c r="B9" s="66"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="51" t="s">
         <v>176</v>
       </c>
@@ -2732,9 +3116,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2744,4 +3128,133 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC1D336-9D64-4429-8CDB-FA9C7AC22479}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="74" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="75" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="75" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="76" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="47">
+        <v>1</v>
+      </c>
+      <c r="B2" s="82" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="77" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="78" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="48">
+        <v>2</v>
+      </c>
+      <c r="B3" s="84"/>
+      <c r="C3" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="50">
+        <v>3</v>
+      </c>
+      <c r="B4" s="83"/>
+      <c r="C4" s="51" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="47">
+        <v>4</v>
+      </c>
+      <c r="B5" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="50">
+        <v>5</v>
+      </c>
+      <c r="B6" s="72"/>
+      <c r="C6" s="73" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="47">
+        <v>6</v>
+      </c>
+      <c r="B7" s="71" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="79" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="50">
+        <v>7</v>
+      </c>
+      <c r="B8" s="72"/>
+      <c r="C8" s="80" t="s">
+        <v>182</v>
+      </c>
+      <c r="D8" s="81" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B2:B4"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Planilha de Requisitos atualizada, arrumada e revisada
</commit_message>
<xml_diff>
--- a/Documentação/planilha requisitos.xlsx
+++ b/Documentação/planilha requisitos.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ultim\Desktop\BandTec\git\boxzard\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9B3665-B6F1-4630-8EC2-BAC73C1B2FC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FA249B-B7EA-4D8E-9AD0-5BF76B117445}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{62812CE9-B7D2-4317-BEDF-1A63102B2E36}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548" firstSheet="1" activeTab="4" xr2:uid="{62812CE9-B7D2-4317-BEDF-1A63102B2E36}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
     <sheet name="Planilha de Requisitos" sheetId="1" r:id="rId2"/>
     <sheet name="Sprint BandTec (2°)" sheetId="5" r:id="rId3"/>
     <sheet name="Sprint Backlog (29-03)" sheetId="3" r:id="rId4"/>
-    <sheet name="Sprint Backlog (05-04)" sheetId="4" r:id="rId5"/>
+    <sheet name="Sprint Backlog (04-04)" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Planilha de Requisitos'!$A$1:$E$7</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="219">
   <si>
     <t>id</t>
   </si>
@@ -127,21 +127,12 @@
     <t>Sensor de umidade para medir a temperatura dos galpões usados para armazenas produtos críticos.</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
     <t>Fazer login para acessar seus dados e informações sobre o serviço contratado.</t>
   </si>
   <si>
-    <t>Notificações</t>
-  </si>
-  <si>
     <t>Gerar relatório sobre as informações desejadas sobre o serviço contratado e os dados que o envolvem.</t>
   </si>
   <si>
-    <t>Gerar Relatório</t>
-  </si>
-  <si>
     <t>RF008</t>
   </si>
   <si>
@@ -331,9 +322,6 @@
     <t>Enviar notificação em caso de mudanças bruscas de temperatura.</t>
   </si>
   <si>
-    <t>Ler Temperatura e Umidade</t>
-  </si>
-  <si>
     <t>Buscar dados de temperatura e umidade ideais no banco de dados.</t>
   </si>
   <si>
@@ -343,15 +331,9 @@
     <t>Compara a temperatura e umidade lida dos sensores com a do banco.</t>
   </si>
   <si>
-    <t>Menu de navegação</t>
-  </si>
-  <si>
     <t>Menu no topo da página do site com os botões - Página Inicial, Sobre, Produto, Simulador Financeiro, Fale Conosco e Login.</t>
   </si>
   <si>
-    <t>Imagem de fundo</t>
-  </si>
-  <si>
     <t>Imagem de fundo na página inicial.</t>
   </si>
   <si>
@@ -361,18 +343,9 @@
     <t>Centralizado na página inicial.</t>
   </si>
   <si>
-    <t>Sobre Nós</t>
-  </si>
-  <si>
     <t>Descrição da empresa contendo história, missão, visão e valores.</t>
   </si>
   <si>
-    <t>Video explicativo</t>
-  </si>
-  <si>
-    <t>Video explicativo do produto.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Informações sobre o produto </t>
   </si>
   <si>
@@ -382,15 +355,9 @@
     <t>Requisitos minimos para o funcionamento do produto.</t>
   </si>
   <si>
-    <t>Calculo de sensores</t>
-  </si>
-  <si>
     <t>Calculo usado para definir a quantidade de sensores necessarios para o funcionamento ideal do produto.</t>
   </si>
   <si>
-    <t>Calculo de pontencia</t>
-  </si>
-  <si>
     <t>Calcular pontência necessária dos ar-condicionados.</t>
   </si>
   <si>
@@ -400,9 +367,6 @@
     <t>Botão para redirecionar o cliente para se cadastrar.</t>
   </si>
   <si>
-    <t>Cadastrar</t>
-  </si>
-  <si>
     <t>Fazer cadastro do cliente.</t>
   </si>
   <si>
@@ -412,36 +376,21 @@
     <t>Escolher forma de pagamento.</t>
   </si>
   <si>
-    <t>Selecionar galpões</t>
-  </si>
-  <si>
     <t>Selecionar quantidade de galpões na hora do cadastro.</t>
   </si>
   <si>
-    <t>Tamanho dos galpões</t>
-  </si>
-  <si>
     <t>Determinar tamanho em metros quadrados.</t>
   </si>
   <si>
-    <t>Quantidade de ar</t>
-  </si>
-  <si>
     <t>Numero de ar-condicionados no local.</t>
   </si>
   <si>
-    <t>Endereço por CEP</t>
-  </si>
-  <si>
     <t>Preenchimento automático a partir do Correios.</t>
   </si>
   <si>
     <t>Formulário para contato. (Que será enviado para o email da empresa)</t>
   </si>
   <si>
-    <t>Tela de gráficos</t>
-  </si>
-  <si>
     <t>Tela contendo métricas, estatisticas e dashboards.</t>
   </si>
   <si>
@@ -451,27 +400,15 @@
     <t>Escolha o periodo para exibição do gráfico. (Diário, semanal, mensal).</t>
   </si>
   <si>
-    <t>Serviços</t>
-  </si>
-  <si>
     <t>Visualizar serviço contratado. (Ver estado dos galpões, produto armazenado e temperatura e umidade ambiente atual).</t>
   </si>
   <si>
-    <t>Perfil do Usuário</t>
-  </si>
-  <si>
     <t>Exibir e editar informaçoes pessoais.</t>
   </si>
   <si>
-    <t>Editar galpão</t>
-  </si>
-  <si>
     <t>Alteração de galpão, produto e temperatura e umidade ideais de forma manual. (Na tela de serviços)</t>
   </si>
   <si>
-    <t>Solicitar reparos</t>
-  </si>
-  <si>
     <t>Solicitar reparos do produto na tela de serviços.</t>
   </si>
   <si>
@@ -484,15 +421,9 @@
     <t>Sensor para transmitir informações entre o arduino e o ar-condicionado.</t>
   </si>
   <si>
-    <t>Validação de email</t>
-  </si>
-  <si>
     <t>Validar cadastro por email.</t>
   </si>
   <si>
-    <t>Excesso de tentativas</t>
-  </si>
-  <si>
     <t>Exceder tentativas de login (Máximo 10).</t>
   </si>
   <si>
@@ -559,36 +490,9 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Menu</t>
-  </si>
-  <si>
-    <t>Contato</t>
-  </si>
-  <si>
-    <t>Criação de tabelas</t>
-  </si>
-  <si>
-    <t>Modelo Conceitual</t>
-  </si>
-  <si>
-    <t>Testar banco de dados</t>
-  </si>
-  <si>
-    <t>Banco de dados inserido no Azure</t>
-  </si>
-  <si>
-    <t>Cadastro</t>
-  </si>
-  <si>
     <t>Arquitetura</t>
   </si>
   <si>
-    <t>HLD</t>
-  </si>
-  <si>
-    <t>LLD</t>
-  </si>
-  <si>
     <t>Prof. Fernando</t>
   </si>
   <si>
@@ -653,6 +557,144 @@
   </si>
   <si>
     <t>Concluido</t>
+  </si>
+  <si>
+    <t>Fazer página Inicial do site Institucional</t>
+  </si>
+  <si>
+    <t>Fazer barra de menu navegação do site</t>
+  </si>
+  <si>
+    <t>Fazer página sobre, que terá informações sobre a empresa como história, missão, visão e valores.</t>
+  </si>
+  <si>
+    <t>Fazer página simulador financeiro onde terá uma simulação de economia ao utilizar nosso software.</t>
+  </si>
+  <si>
+    <t>Página produto onde terá informações mais detalhadas sobre o projeto e o produto que será oferecido.</t>
+  </si>
+  <si>
+    <t>Página contato onde poderá encontrar informações como telefone, endereço e enviar uma mensagem para nós.</t>
+  </si>
+  <si>
+    <t>Criar tabelas no banco de dados local.</t>
+  </si>
+  <si>
+    <t>Criar modelo conceitual do banco de dados no BrModelo.</t>
+  </si>
+  <si>
+    <t>Finalizar simulador financeiro do site.</t>
+  </si>
+  <si>
+    <t>Testar banco de dados local.</t>
+  </si>
+  <si>
+    <t>Criar tabelas do banco de dados no Azure.</t>
+  </si>
+  <si>
+    <t>Criar arquitetura HLD do projeto.</t>
+  </si>
+  <si>
+    <t>Criar arquitetura LLD do projeto.</t>
+  </si>
+  <si>
+    <t>Registrar dados vindos do Arduino</t>
+  </si>
+  <si>
+    <t>Buscar dados de ambientação do banco</t>
+  </si>
+  <si>
+    <t>Comparar estado do ambiente atual com a ideal do banco de dados</t>
+  </si>
+  <si>
+    <t>Adaptar ambiente para a ideal descrita no banco de dados</t>
+  </si>
+  <si>
+    <t>Registrar dados de mudanças de temperatura e umidade</t>
+  </si>
+  <si>
+    <t>Ler Temperatura e Umidade do ambiente</t>
+  </si>
+  <si>
+    <t>Menu de navegação do site</t>
+  </si>
+  <si>
+    <t>Site terá a função de login</t>
+  </si>
+  <si>
+    <t>Imagem de fundo para tela inicial</t>
+  </si>
+  <si>
+    <t>Página contando um pouco sobre nós</t>
+  </si>
+  <si>
+    <t>Video explicativo sobre o produto</t>
+  </si>
+  <si>
+    <t>Video explicativo do produto com informações técnicas e suas funcionalidades.</t>
+  </si>
+  <si>
+    <t>Sessão para descrever as premissas do produto</t>
+  </si>
+  <si>
+    <t>Página do simulador financeiro</t>
+  </si>
+  <si>
+    <t>Cadastrar clientes na base de dados</t>
+  </si>
+  <si>
+    <t>Calcular quantidade de sensores</t>
+  </si>
+  <si>
+    <t>Calcular pontencia dos ar-condicionados</t>
+  </si>
+  <si>
+    <t>Selecionar quantidade de galpões que o cliente possui</t>
+  </si>
+  <si>
+    <t>Campo para informar o tamanho dos galpões</t>
+  </si>
+  <si>
+    <t>Campo para informar a quantidade de ar condicionados no galpão</t>
+  </si>
+  <si>
+    <t>Campo para inserir o endereço por CEP</t>
+  </si>
+  <si>
+    <t>Função de validação de email</t>
+  </si>
+  <si>
+    <t>Função para excesso de tentativas de login</t>
+  </si>
+  <si>
+    <t>Sessão de fale Conosco</t>
+  </si>
+  <si>
+    <t>Sessão de tela de gráficos no perfil do cliente</t>
+  </si>
+  <si>
+    <t>Sessão de serviços</t>
+  </si>
+  <si>
+    <t>Sessão para solicitar reparos</t>
+  </si>
+  <si>
+    <t>Sessão com campos onde será possivel a edição das informações dos galpões</t>
+  </si>
+  <si>
+    <t>Função de notificações no site para o cliente</t>
+  </si>
+  <si>
+    <t>Função para gerar relatório das informações contidas no site</t>
+  </si>
+  <si>
+    <t>Sessão perfil do usuário</t>
+  </si>
+  <si>
+    <t>Criar tela de login do usuário com os campos: Email e senha, e dois botões: Entrar e cadastrar.</t>
+  </si>
+  <si>
+    <t>Criar tela de cadastro de usuário com os campos: Nome completo, CPF/CNPJ, CEP, numero, complemento, email, senha, telefone de contato, qtd de galpões, metros quadrados dos galpões, qtd de ar condicionados e potencia dos ar-condicionados.</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1227,9 +1269,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1250,7 +1289,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1258,14 +1296,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
@@ -1273,64 +1306,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1350,6 +1336,69 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1666,23 +1715,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809286DD-D5C9-4F7B-AD94-6A53F56382A7}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>7</v>
@@ -1691,144 +1740,144 @@
         <v>2</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="24">
         <v>1</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="83" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E2" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="63"/>
+      <c r="B3" s="84"/>
       <c r="C3" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E3" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="63"/>
+      <c r="B4" s="84"/>
       <c r="C4" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E4" s="18">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="63"/>
+      <c r="B5" s="84"/>
       <c r="C5" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E5" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="63"/>
+      <c r="B6" s="84"/>
       <c r="C6" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E6" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>6</v>
       </c>
-      <c r="B7" s="63"/>
+      <c r="B7" s="84"/>
       <c r="C7" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E7" s="18">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>7</v>
       </c>
-      <c r="B8" s="63"/>
+      <c r="B8" s="84"/>
       <c r="C8" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E8" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="20">
         <v>8</v>
       </c>
-      <c r="B9" s="64"/>
+      <c r="B9" s="85"/>
       <c r="C9" s="21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E9" s="23">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
       <c r="D10" s="4"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>7</v>
@@ -1837,138 +1886,138 @@
         <v>2</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>9</v>
       </c>
-      <c r="B12" s="62" t="s">
-        <v>67</v>
+      <c r="B12" s="83" t="s">
+        <v>64</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E12" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <v>10</v>
       </c>
-      <c r="B13" s="63"/>
+      <c r="B13" s="84"/>
       <c r="C13" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E13" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>11</v>
       </c>
-      <c r="B14" s="63"/>
+      <c r="B14" s="84"/>
       <c r="C14" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E14" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>12</v>
       </c>
-      <c r="B15" s="63"/>
+      <c r="B15" s="84"/>
       <c r="C15" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E15" s="18">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>13</v>
       </c>
-      <c r="B16" s="63"/>
+      <c r="B16" s="84"/>
       <c r="C16" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E16" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>14</v>
       </c>
-      <c r="B17" s="63"/>
+      <c r="B17" s="84"/>
       <c r="C17" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E17" s="18">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>15</v>
       </c>
-      <c r="B18" s="63"/>
+      <c r="B18" s="84"/>
       <c r="C18" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E18" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="20">
         <v>16</v>
       </c>
-      <c r="B19" s="64"/>
+      <c r="B19" s="85"/>
       <c r="C19" s="21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E19" s="23">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>7</v>
@@ -1977,96 +2026,96 @@
         <v>2</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>17</v>
       </c>
-      <c r="B22" s="62" t="s">
-        <v>82</v>
+      <c r="B22" s="83" t="s">
+        <v>79</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E22" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="17">
         <v>18</v>
       </c>
-      <c r="B23" s="63"/>
+      <c r="B23" s="84"/>
       <c r="C23" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E23" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>19</v>
       </c>
-      <c r="B24" s="63"/>
+      <c r="B24" s="84"/>
       <c r="C24" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E24" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>20</v>
       </c>
-      <c r="B25" s="63"/>
+      <c r="B25" s="84"/>
       <c r="C25" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E25" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>21</v>
       </c>
-      <c r="B26" s="63"/>
+      <c r="B26" s="84"/>
       <c r="C26" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E26" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>22</v>
       </c>
-      <c r="B27" s="63"/>
+      <c r="B27" s="84"/>
       <c r="C27" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E27" s="18">
         <v>4</v>
@@ -2087,655 +2136,655 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1AC4D2-7026-4F35-A980-9AD1E4D216BB}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="43" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="35" t="s">
-        <v>99</v>
+      <c r="C2" s="82" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>95</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="5" t="s">
-        <v>85</v>
+      <c r="B3" s="87"/>
+      <c r="C3" s="6" t="s">
+        <v>186</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="5" t="s">
-        <v>87</v>
+      <c r="B4" s="87"/>
+      <c r="C4" s="6" t="s">
+        <v>187</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="5" t="s">
-        <v>91</v>
+      <c r="B5" s="87"/>
+      <c r="C5" s="6" t="s">
+        <v>188</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="5" t="s">
-        <v>91</v>
+      <c r="B6" s="87"/>
+      <c r="C6" s="6" t="s">
+        <v>189</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="67"/>
+      <c r="B7" s="88"/>
       <c r="C7" s="28" t="s">
-        <v>85</v>
+        <v>190</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E7" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="29"/>
       <c r="B8" s="30"/>
       <c r="C8" s="31"/>
       <c r="D8" s="32"/>
       <c r="E8" s="29"/>
     </row>
-    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="86" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>101</v>
+        <v>192</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="87"/>
+      <c r="C10" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="D10" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="37" t="s">
-        <v>30</v>
-      </c>
       <c r="E10" s="18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="5" t="s">
-        <v>103</v>
+      <c r="B11" s="87"/>
+      <c r="C11" s="6" t="s">
+        <v>194</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="B12" s="66"/>
+        <v>129</v>
+      </c>
+      <c r="B12" s="87"/>
       <c r="C12" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="5" t="s">
-        <v>107</v>
+        <v>130</v>
+      </c>
+      <c r="B13" s="87"/>
+      <c r="C13" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="5" t="s">
-        <v>109</v>
+        <v>32</v>
+      </c>
+      <c r="B14" s="87"/>
+      <c r="C14" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>110</v>
+        <v>197</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="66"/>
+        <v>33</v>
+      </c>
+      <c r="B15" s="87"/>
       <c r="C15" s="6" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="66"/>
+        <v>34</v>
+      </c>
+      <c r="B16" s="87"/>
       <c r="C16" s="6" t="s">
-        <v>59</v>
+        <v>198</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="66"/>
+        <v>35</v>
+      </c>
+      <c r="B17" s="87"/>
       <c r="C17" s="6" t="s">
-        <v>57</v>
+        <v>199</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="66"/>
+        <v>36</v>
+      </c>
+      <c r="B18" s="87"/>
       <c r="C18" s="6" t="s">
-        <v>114</v>
+        <v>201</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="66"/>
+        <v>42</v>
+      </c>
+      <c r="B19" s="87"/>
       <c r="C19" s="6" t="s">
-        <v>116</v>
+        <v>202</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="66"/>
+        <v>43</v>
+      </c>
+      <c r="B20" s="87"/>
       <c r="C20" s="6" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="B21" s="66"/>
+        <v>131</v>
+      </c>
+      <c r="B21" s="87"/>
       <c r="C21" s="6" t="s">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="B22" s="66"/>
+        <v>132</v>
+      </c>
+      <c r="B22" s="87"/>
       <c r="C22" s="6" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="B23" s="66"/>
+        <v>133</v>
+      </c>
+      <c r="B23" s="87"/>
       <c r="C23" s="6" t="s">
-        <v>124</v>
+        <v>203</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="B24" s="66"/>
+        <v>134</v>
+      </c>
+      <c r="B24" s="87"/>
       <c r="C24" s="6" t="s">
-        <v>126</v>
+        <v>204</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="B25" s="66"/>
+        <v>135</v>
+      </c>
+      <c r="B25" s="87"/>
       <c r="C25" s="6" t="s">
-        <v>128</v>
+        <v>205</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="B26" s="66"/>
+        <v>136</v>
+      </c>
+      <c r="B26" s="87"/>
       <c r="C26" s="6" t="s">
-        <v>130</v>
+        <v>206</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="B27" s="66"/>
+        <v>137</v>
+      </c>
+      <c r="B27" s="87"/>
       <c r="C27" s="6" t="s">
-        <v>148</v>
+        <v>207</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="E27" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="B28" s="66"/>
+        <v>138</v>
+      </c>
+      <c r="B28" s="87"/>
       <c r="C28" s="6" t="s">
-        <v>150</v>
+        <v>208</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="B29" s="66"/>
+        <v>139</v>
+      </c>
+      <c r="B29" s="87"/>
       <c r="C29" s="6" t="s">
-        <v>63</v>
+        <v>209</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="E29" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="B30" s="66"/>
+        <v>140</v>
+      </c>
+      <c r="B30" s="87"/>
       <c r="C30" s="6" t="s">
-        <v>133</v>
+        <v>210</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="B31" s="66"/>
-      <c r="C31" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="D31" s="37" t="s">
-        <v>136</v>
+        <v>141</v>
+      </c>
+      <c r="B31" s="87"/>
+      <c r="C31" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>119</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="B32" s="66"/>
+        <v>142</v>
+      </c>
+      <c r="B32" s="87"/>
       <c r="C32" s="5" t="s">
-        <v>137</v>
+        <v>211</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="B33" s="66"/>
-      <c r="C33" s="5" t="s">
-        <v>141</v>
+        <v>143</v>
+      </c>
+      <c r="B33" s="87"/>
+      <c r="C33" s="6" t="s">
+        <v>213</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="B34" s="66"/>
+        <v>144</v>
+      </c>
+      <c r="B34" s="87"/>
       <c r="C34" s="5" t="s">
-        <v>143</v>
+        <v>212</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="E34" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="B35" s="66"/>
-      <c r="C35" s="5" t="s">
-        <v>31</v>
+        <v>145</v>
+      </c>
+      <c r="B35" s="87"/>
+      <c r="C35" s="6" t="s">
+        <v>214</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E35" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="B36" s="66"/>
+        <v>146</v>
+      </c>
+      <c r="B36" s="87"/>
       <c r="C36" s="6" t="s">
-        <v>33</v>
+        <v>215</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E36" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="B37" s="67"/>
+        <v>147</v>
+      </c>
+      <c r="B37" s="88"/>
       <c r="C37" s="28" t="s">
-        <v>139</v>
+        <v>216</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="E37" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="29"/>
       <c r="B38" s="30"/>
       <c r="C38" s="31"/>
       <c r="D38" s="32"/>
       <c r="E38" s="29"/>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="65" t="s">
-        <v>40</v>
+      <c r="B39" s="86" t="s">
+        <v>37</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="66"/>
+      <c r="B40" s="87"/>
       <c r="C40" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="67"/>
+      <c r="B41" s="88"/>
       <c r="C41" s="21" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="29"/>
       <c r="B42" s="30"/>
-      <c r="C42" s="38"/>
+      <c r="C42" s="37"/>
       <c r="D42" s="32"/>
       <c r="E42" s="29"/>
     </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="65" t="s">
+      <c r="B43" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="C43" s="39" t="s">
-        <v>146</v>
+      <c r="C43" s="38" t="s">
+        <v>125</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="66"/>
+        <v>41</v>
+      </c>
+      <c r="B44" s="87"/>
       <c r="C44" s="5" t="s">
         <v>17</v>
       </c>
@@ -2743,14 +2792,14 @@
         <v>18</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="B45" s="67"/>
+        <v>148</v>
+      </c>
+      <c r="B45" s="88"/>
       <c r="C45" s="28" t="s">
         <v>25</v>
       </c>
@@ -2758,7 +2807,7 @@
         <v>28</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2785,191 +2834,191 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="58" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="65" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="45">
+        <v>1</v>
+      </c>
+      <c r="B2" s="89" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="66" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="68" t="s">
         <v>172</v>
       </c>
-      <c r="B1" s="75" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="75" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="48">
         <v>2</v>
       </c>
-      <c r="D1" s="87" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="47">
-        <v>1</v>
-      </c>
-      <c r="B2" s="86" t="s">
-        <v>183</v>
-      </c>
-      <c r="C2" s="88" t="s">
-        <v>184</v>
-      </c>
-      <c r="D2" s="90" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50">
-        <v>2</v>
-      </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="89" t="s">
-        <v>185</v>
-      </c>
-      <c r="D3" s="93" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="33" x14ac:dyDescent="0.25">
-      <c r="A4" s="47">
+      <c r="B3" s="90"/>
+      <c r="C3" s="67" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="71" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="45">
         <v>3</v>
       </c>
-      <c r="B4" s="86" t="s">
-        <v>186</v>
-      </c>
-      <c r="C4" s="88" t="s">
-        <v>187</v>
-      </c>
-      <c r="D4" s="96" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="33" x14ac:dyDescent="0.25">
-      <c r="A5" s="48">
+      <c r="B4" s="89" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="74" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="46">
         <v>4</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="85" t="s">
-        <v>188</v>
-      </c>
-      <c r="D5" s="94" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50">
+      <c r="B5" s="91"/>
+      <c r="C5" s="64" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="72" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="48">
         <v>5</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="89" t="s">
-        <v>189</v>
-      </c>
-      <c r="D6" s="97" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="33" x14ac:dyDescent="0.25">
-      <c r="A7" s="47">
+      <c r="B6" s="90"/>
+      <c r="C6" s="67" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="75" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="45">
         <v>6</v>
       </c>
-      <c r="B7" s="86" t="s">
-        <v>190</v>
-      </c>
-      <c r="C7" s="88" t="s">
-        <v>191</v>
-      </c>
-      <c r="D7" s="91" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="33" x14ac:dyDescent="0.25">
-      <c r="A8" s="48">
+      <c r="B7" s="89" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="69" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="46">
         <v>7</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="85" t="s">
-        <v>192</v>
-      </c>
-      <c r="D8" s="98" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50">
+      <c r="B8" s="91"/>
+      <c r="C8" s="64" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" s="76" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="48">
         <v>8</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="89" t="s">
-        <v>193</v>
-      </c>
-      <c r="D9" s="92" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="33" x14ac:dyDescent="0.25">
-      <c r="A10" s="47">
+      <c r="B9" s="90"/>
+      <c r="C9" s="67" t="s">
+        <v>161</v>
+      </c>
+      <c r="D9" s="70" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="45">
         <v>9</v>
       </c>
-      <c r="B10" s="86" t="s">
-        <v>194</v>
-      </c>
-      <c r="C10" s="88" t="s">
-        <v>195</v>
-      </c>
-      <c r="D10" s="91" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="50">
+      <c r="B10" s="89" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>163</v>
+      </c>
+      <c r="D10" s="69" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="51" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="48">
         <v>10</v>
       </c>
-      <c r="B11" s="70"/>
-      <c r="C11" s="89" t="s">
-        <v>196</v>
-      </c>
-      <c r="D11" s="97" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="47">
+      <c r="B11" s="90"/>
+      <c r="C11" s="67" t="s">
+        <v>164</v>
+      </c>
+      <c r="D11" s="75" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="45">
         <v>11</v>
       </c>
-      <c r="B12" s="86" t="s">
-        <v>197</v>
-      </c>
-      <c r="C12" s="88" t="s">
-        <v>198</v>
-      </c>
-      <c r="D12" s="95" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="33" x14ac:dyDescent="0.25">
-      <c r="A13" s="48">
+      <c r="B12" s="89" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" s="73" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="46">
         <v>12</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="85" t="s">
-        <v>199</v>
-      </c>
-      <c r="D13" s="94" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="50">
+      <c r="B13" s="91"/>
+      <c r="C13" s="64" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="72" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="48">
         <v>13</v>
       </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="89" t="s">
-        <v>200</v>
-      </c>
-      <c r="D14" s="93" t="s">
-        <v>202</v>
+      <c r="B14" s="90"/>
+      <c r="C14" s="67" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="71" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2991,134 +3040,134 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="B1" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="60" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="54" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="56" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="57">
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="52">
         <v>1</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="58" t="s">
+      <c r="C2" s="77" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="46"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="48">
+      <c r="F2" s="44"/>
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="46">
         <v>2</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="45" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3" s="49" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="48">
+      <c r="B3" s="91"/>
+      <c r="C3" s="78" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="46">
         <v>3</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="49" t="s">
+      <c r="B4" s="91"/>
+      <c r="C4" s="78" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" s="47" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="48">
+    <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="46">
         <v>4</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="49" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="48">
+      <c r="B5" s="91"/>
+      <c r="C5" s="78" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="46">
         <v>5</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="49" t="s">
+      <c r="B6" s="91"/>
+      <c r="C6" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="D6" s="47" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="50">
+    <row r="7" spans="1:6" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="48">
         <v>6</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="51" t="s">
-        <v>174</v>
-      </c>
-      <c r="D7" s="52" t="s">
+      <c r="B7" s="90"/>
+      <c r="C7" s="57" t="s">
+        <v>178</v>
+      </c>
+      <c r="D7" s="49" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47">
+    <row r="8" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="45">
         <v>8</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="55" t="s">
-        <v>175</v>
-      </c>
-      <c r="D8" s="56" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50">
+      <c r="C8" s="79" t="s">
+        <v>179</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="48">
         <v>7</v>
       </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="51" t="s">
-        <v>176</v>
-      </c>
-      <c r="D9" s="52" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="57" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3134,118 +3183,118 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC1D336-9D64-4429-8CDB-FA9C7AC22479}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="74" t="s">
-        <v>172</v>
-      </c>
-      <c r="B1" s="75" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="75" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="58" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="60" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="47">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="45">
         <v>1</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="77" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="78" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="48">
+      <c r="C2" s="80" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" s="61" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="46">
         <v>2</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="49" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50">
+      <c r="B3" s="96"/>
+      <c r="C3" s="78" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="48">
         <v>3</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="51" t="s">
-        <v>179</v>
-      </c>
-      <c r="D4" s="52" t="s">
+      <c r="B4" s="97"/>
+      <c r="C4" s="57" t="s">
+        <v>218</v>
+      </c>
+      <c r="D4" s="49" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="47">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="45">
         <v>4</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="55" t="s">
-        <v>177</v>
-      </c>
-      <c r="D5" s="56" t="s">
+      <c r="C5" s="79" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="51" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50">
+    <row r="6" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="48">
         <v>5</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="73" t="s">
-        <v>178</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="47">
+      <c r="B6" s="94"/>
+      <c r="C6" s="57" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="45">
         <v>6</v>
       </c>
-      <c r="B7" s="71" t="s">
-        <v>180</v>
-      </c>
-      <c r="C7" s="79" t="s">
-        <v>181</v>
-      </c>
-      <c r="D7" s="56" t="s">
+      <c r="B7" s="93" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="81" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" s="51" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="50">
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="48">
         <v>7</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="80" t="s">
-        <v>182</v>
-      </c>
-      <c r="D8" s="81" t="s">
+      <c r="B8" s="94"/>
+      <c r="C8" s="62" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8" s="63" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adição do simulador e aprimoramento da sessão produto
</commit_message>
<xml_diff>
--- a/Documentação/planilha requisitos.xlsx
+++ b/Documentação/planilha requisitos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ultim\Desktop\BandTec\git\boxzard\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FA249B-B7EA-4D8E-9AD0-5BF76B117445}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9649F64A-9A52-4231-9E71-022D0C08EB13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548" firstSheet="1" activeTab="4" xr2:uid="{62812CE9-B7D2-4317-BEDF-1A63102B2E36}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="1" activeTab="4" xr2:uid="{62812CE9-B7D2-4317-BEDF-1A63102B2E36}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
@@ -1313,7 +1313,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1398,6 +1397,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1719,14 +1721,14 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -1743,11 +1745,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="24">
         <v>1</v>
       </c>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="82" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="14" t="s">
@@ -1760,11 +1762,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="84"/>
+      <c r="B3" s="83"/>
       <c r="C3" s="5" t="s">
         <v>50</v>
       </c>
@@ -1775,11 +1777,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="84"/>
+      <c r="B4" s="83"/>
       <c r="C4" s="5" t="s">
         <v>51</v>
       </c>
@@ -1790,11 +1792,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="84"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="5" t="s">
         <v>54</v>
       </c>
@@ -1805,11 +1807,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="84"/>
+      <c r="B6" s="83"/>
       <c r="C6" s="5" t="s">
         <v>56</v>
       </c>
@@ -1820,11 +1822,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>6</v>
       </c>
-      <c r="B7" s="84"/>
+      <c r="B7" s="83"/>
       <c r="C7" s="6" t="s">
         <v>58</v>
       </c>
@@ -1835,11 +1837,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>7</v>
       </c>
-      <c r="B8" s="84"/>
+      <c r="B8" s="83"/>
       <c r="C8" s="5" t="s">
         <v>60</v>
       </c>
@@ -1850,11 +1852,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20">
         <v>8</v>
       </c>
-      <c r="B9" s="85"/>
+      <c r="B9" s="84"/>
       <c r="C9" s="21" t="s">
         <v>62</v>
       </c>
@@ -1865,14 +1867,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
       <c r="D10" s="4"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -1889,11 +1891,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>9</v>
       </c>
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="82" t="s">
         <v>64</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -1906,11 +1908,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>10</v>
       </c>
-      <c r="B13" s="84"/>
+      <c r="B13" s="83"/>
       <c r="C13" s="5" t="s">
         <v>67</v>
       </c>
@@ -1921,11 +1923,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>11</v>
       </c>
-      <c r="B14" s="84"/>
+      <c r="B14" s="83"/>
       <c r="C14" s="5" t="s">
         <v>69</v>
       </c>
@@ -1936,11 +1938,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>12</v>
       </c>
-      <c r="B15" s="84"/>
+      <c r="B15" s="83"/>
       <c r="C15" s="5" t="s">
         <v>71</v>
       </c>
@@ -1951,11 +1953,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>13</v>
       </c>
-      <c r="B16" s="84"/>
+      <c r="B16" s="83"/>
       <c r="C16" s="5" t="s">
         <v>77</v>
       </c>
@@ -1966,11 +1968,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>14</v>
       </c>
-      <c r="B17" s="84"/>
+      <c r="B17" s="83"/>
       <c r="C17" s="6" t="s">
         <v>73</v>
       </c>
@@ -1981,11 +1983,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>15</v>
       </c>
-      <c r="B18" s="84"/>
+      <c r="B18" s="83"/>
       <c r="C18" s="5" t="s">
         <v>92</v>
       </c>
@@ -1996,11 +1998,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20">
         <v>16</v>
       </c>
-      <c r="B19" s="85"/>
+      <c r="B19" s="84"/>
       <c r="C19" s="21" t="s">
         <v>75</v>
       </c>
@@ -2011,8 +2013,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>0</v>
       </c>
@@ -2029,11 +2031,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>17</v>
       </c>
-      <c r="B22" s="83" t="s">
+      <c r="B22" s="82" t="s">
         <v>79</v>
       </c>
       <c r="C22" s="14" t="s">
@@ -2046,11 +2048,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>18</v>
       </c>
-      <c r="B23" s="84"/>
+      <c r="B23" s="83"/>
       <c r="C23" s="5" t="s">
         <v>82</v>
       </c>
@@ -2061,11 +2063,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>19</v>
       </c>
-      <c r="B24" s="84"/>
+      <c r="B24" s="83"/>
       <c r="C24" s="5" t="s">
         <v>84</v>
       </c>
@@ -2076,11 +2078,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>20</v>
       </c>
-      <c r="B25" s="84"/>
+      <c r="B25" s="83"/>
       <c r="C25" s="5" t="s">
         <v>86</v>
       </c>
@@ -2091,11 +2093,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>21</v>
       </c>
-      <c r="B26" s="84"/>
+      <c r="B26" s="83"/>
       <c r="C26" s="5" t="s">
         <v>88</v>
       </c>
@@ -2106,11 +2108,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="19">
         <v>22</v>
       </c>
-      <c r="B27" s="84"/>
+      <c r="B27" s="83"/>
       <c r="C27" s="6" t="s">
         <v>90</v>
       </c>
@@ -2140,14 +2142,14 @@
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -2164,14 +2166,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="81" t="s">
         <v>191</v>
       </c>
       <c r="D2" s="34" t="s">
@@ -2181,11 +2183,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="87"/>
+      <c r="B3" s="86"/>
       <c r="C3" s="6" t="s">
         <v>186</v>
       </c>
@@ -2197,11 +2199,11 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="87"/>
+      <c r="B4" s="86"/>
       <c r="C4" s="6" t="s">
         <v>187</v>
       </c>
@@ -2213,11 +2215,11 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="87"/>
+      <c r="B5" s="86"/>
       <c r="C5" s="6" t="s">
         <v>188</v>
       </c>
@@ -2228,11 +2230,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="87"/>
+      <c r="B6" s="86"/>
       <c r="C6" s="6" t="s">
         <v>189</v>
       </c>
@@ -2243,11 +2245,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="88"/>
+      <c r="B7" s="87"/>
       <c r="C7" s="28" t="s">
         <v>190</v>
       </c>
@@ -2258,18 +2260,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29"/>
       <c r="B8" s="30"/>
       <c r="C8" s="31"/>
       <c r="D8" s="32"/>
       <c r="E8" s="29"/>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="85" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="33" t="s">
@@ -2282,11 +2284,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="87"/>
+      <c r="B10" s="86"/>
       <c r="C10" s="35" t="s">
         <v>193</v>
       </c>
@@ -2297,11 +2299,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="87"/>
+      <c r="B11" s="86"/>
       <c r="C11" s="6" t="s">
         <v>194</v>
       </c>
@@ -2312,11 +2314,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="87"/>
+      <c r="B12" s="86"/>
       <c r="C12" s="5" t="s">
         <v>99</v>
       </c>
@@ -2327,11 +2329,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="87"/>
+      <c r="B13" s="86"/>
       <c r="C13" s="6" t="s">
         <v>195</v>
       </c>
@@ -2342,11 +2344,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="87"/>
+      <c r="B14" s="86"/>
       <c r="C14" s="6" t="s">
         <v>196</v>
       </c>
@@ -2357,11 +2359,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="87"/>
+      <c r="B15" s="86"/>
       <c r="C15" s="6" t="s">
         <v>102</v>
       </c>
@@ -2372,11 +2374,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="87"/>
+      <c r="B16" s="86"/>
       <c r="C16" s="6" t="s">
         <v>198</v>
       </c>
@@ -2387,11 +2389,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="87"/>
+      <c r="B17" s="86"/>
       <c r="C17" s="6" t="s">
         <v>199</v>
       </c>
@@ -2402,11 +2404,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="87"/>
+      <c r="B18" s="86"/>
       <c r="C18" s="6" t="s">
         <v>201</v>
       </c>
@@ -2417,11 +2419,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="87"/>
+      <c r="B19" s="86"/>
       <c r="C19" s="6" t="s">
         <v>202</v>
       </c>
@@ -2432,11 +2434,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="87"/>
+      <c r="B20" s="86"/>
       <c r="C20" s="6" t="s">
         <v>107</v>
       </c>
@@ -2447,11 +2449,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="B21" s="87"/>
+      <c r="B21" s="86"/>
       <c r="C21" s="6" t="s">
         <v>200</v>
       </c>
@@ -2462,11 +2464,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="B22" s="87"/>
+      <c r="B22" s="86"/>
       <c r="C22" s="6" t="s">
         <v>110</v>
       </c>
@@ -2477,11 +2479,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="B23" s="87"/>
+      <c r="B23" s="86"/>
       <c r="C23" s="6" t="s">
         <v>203</v>
       </c>
@@ -2492,11 +2494,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="B24" s="87"/>
+      <c r="B24" s="86"/>
       <c r="C24" s="6" t="s">
         <v>204</v>
       </c>
@@ -2507,11 +2509,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="B25" s="87"/>
+      <c r="B25" s="86"/>
       <c r="C25" s="6" t="s">
         <v>205</v>
       </c>
@@ -2522,11 +2524,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="B26" s="87"/>
+      <c r="B26" s="86"/>
       <c r="C26" s="6" t="s">
         <v>206</v>
       </c>
@@ -2537,11 +2539,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B27" s="87"/>
+      <c r="B27" s="86"/>
       <c r="C27" s="6" t="s">
         <v>207</v>
       </c>
@@ -2552,11 +2554,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B28" s="87"/>
+      <c r="B28" s="86"/>
       <c r="C28" s="6" t="s">
         <v>208</v>
       </c>
@@ -2567,11 +2569,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="B29" s="87"/>
+      <c r="B29" s="86"/>
       <c r="C29" s="6" t="s">
         <v>209</v>
       </c>
@@ -2582,11 +2584,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="B30" s="87"/>
+      <c r="B30" s="86"/>
       <c r="C30" s="6" t="s">
         <v>210</v>
       </c>
@@ -2597,11 +2599,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="B31" s="87"/>
+      <c r="B31" s="86"/>
       <c r="C31" s="35" t="s">
         <v>118</v>
       </c>
@@ -2612,11 +2614,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="B32" s="87"/>
+      <c r="B32" s="86"/>
       <c r="C32" s="5" t="s">
         <v>211</v>
       </c>
@@ -2627,11 +2629,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="B33" s="87"/>
+      <c r="B33" s="86"/>
       <c r="C33" s="6" t="s">
         <v>213</v>
       </c>
@@ -2642,11 +2644,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="B34" s="87"/>
+      <c r="B34" s="86"/>
       <c r="C34" s="5" t="s">
         <v>212</v>
       </c>
@@ -2657,11 +2659,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="B35" s="87"/>
+      <c r="B35" s="86"/>
       <c r="C35" s="6" t="s">
         <v>214</v>
       </c>
@@ -2672,11 +2674,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="B36" s="87"/>
+      <c r="B36" s="86"/>
       <c r="C36" s="6" t="s">
         <v>215</v>
       </c>
@@ -2687,11 +2689,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="B37" s="88"/>
+      <c r="B37" s="87"/>
       <c r="C37" s="28" t="s">
         <v>216</v>
       </c>
@@ -2702,18 +2704,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="29"/>
       <c r="B38" s="30"/>
       <c r="C38" s="31"/>
       <c r="D38" s="32"/>
       <c r="E38" s="29"/>
     </row>
-    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="86" t="s">
+      <c r="B39" s="85" t="s">
         <v>37</v>
       </c>
       <c r="C39" s="14" t="s">
@@ -2726,11 +2728,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="87"/>
+      <c r="B40" s="86"/>
       <c r="C40" s="5" t="s">
         <v>27</v>
       </c>
@@ -2741,11 +2743,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="88"/>
+      <c r="B41" s="87"/>
       <c r="C41" s="21" t="s">
         <v>124</v>
       </c>
@@ -2756,18 +2758,18 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="29"/>
       <c r="B42" s="30"/>
       <c r="C42" s="37"/>
       <c r="D42" s="32"/>
       <c r="E42" s="29"/>
     </row>
-    <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="86" t="s">
+      <c r="B43" s="85" t="s">
         <v>16</v>
       </c>
       <c r="C43" s="38" t="s">
@@ -2780,11 +2782,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="87"/>
+      <c r="B44" s="86"/>
       <c r="C44" s="5" t="s">
         <v>17</v>
       </c>
@@ -2795,11 +2797,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="B45" s="88"/>
+      <c r="B45" s="87"/>
       <c r="C45" s="28" t="s">
         <v>25</v>
       </c>
@@ -2834,14 +2836,14 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="58" t="s">
         <v>149</v>
       </c>
@@ -2851,173 +2853,173 @@
       <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="64" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="50.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A2" s="45">
         <v>1</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="88" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="65" t="s">
         <v>152</v>
       </c>
-      <c r="D2" s="68" t="s">
+      <c r="D2" s="67" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="48">
         <v>2</v>
       </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="67" t="s">
+      <c r="B3" s="89"/>
+      <c r="C3" s="66" t="s">
         <v>153</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="70" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="33" x14ac:dyDescent="0.25">
       <c r="A4" s="45">
         <v>3</v>
       </c>
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="88" t="s">
         <v>154</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="65" t="s">
         <v>155</v>
       </c>
-      <c r="D4" s="74" t="s">
+      <c r="D4" s="73" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="33" x14ac:dyDescent="0.25">
       <c r="A5" s="46">
         <v>4</v>
       </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="64" t="s">
+      <c r="B5" s="90"/>
+      <c r="C5" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="D5" s="72" t="s">
+      <c r="D5" s="71" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="48">
         <v>5</v>
       </c>
-      <c r="B6" s="90"/>
-      <c r="C6" s="67" t="s">
+      <c r="B6" s="89"/>
+      <c r="C6" s="66" t="s">
         <v>157</v>
       </c>
-      <c r="D6" s="75" t="s">
+      <c r="D6" s="74" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="33" x14ac:dyDescent="0.25">
       <c r="A7" s="45">
         <v>6</v>
       </c>
-      <c r="B7" s="89" t="s">
+      <c r="B7" s="88" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="66" t="s">
+      <c r="C7" s="65" t="s">
         <v>159</v>
       </c>
-      <c r="D7" s="69" t="s">
+      <c r="D7" s="68" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="33" x14ac:dyDescent="0.25">
       <c r="A8" s="46">
         <v>7</v>
       </c>
-      <c r="B8" s="91"/>
-      <c r="C8" s="64" t="s">
+      <c r="B8" s="90"/>
+      <c r="C8" s="63" t="s">
         <v>160</v>
       </c>
-      <c r="D8" s="76" t="s">
+      <c r="D8" s="75" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="48">
         <v>8</v>
       </c>
-      <c r="B9" s="90"/>
-      <c r="C9" s="67" t="s">
+      <c r="B9" s="89"/>
+      <c r="C9" s="66" t="s">
         <v>161</v>
       </c>
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="69" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="33" x14ac:dyDescent="0.25">
       <c r="A10" s="45">
         <v>9</v>
       </c>
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="88" t="s">
         <v>162</v>
       </c>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="65" t="s">
         <v>163</v>
       </c>
-      <c r="D10" s="69" t="s">
+      <c r="D10" s="68" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="51" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="48">
         <v>10</v>
       </c>
-      <c r="B11" s="90"/>
-      <c r="C11" s="67" t="s">
+      <c r="B11" s="89"/>
+      <c r="C11" s="66" t="s">
         <v>164</v>
       </c>
-      <c r="D11" s="75" t="s">
+      <c r="D11" s="74" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="50.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A12" s="45">
         <v>11</v>
       </c>
-      <c r="B12" s="89" t="s">
+      <c r="B12" s="88" t="s">
         <v>165</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="65" t="s">
         <v>166</v>
       </c>
-      <c r="D12" s="73" t="s">
+      <c r="D12" s="72" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="33" x14ac:dyDescent="0.25">
       <c r="A13" s="46">
         <v>12</v>
       </c>
-      <c r="B13" s="91"/>
-      <c r="C13" s="64" t="s">
+      <c r="B13" s="90"/>
+      <c r="C13" s="63" t="s">
         <v>167</v>
       </c>
-      <c r="D13" s="72" t="s">
+      <c r="D13" s="71" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="48">
         <v>13</v>
       </c>
-      <c r="B14" s="90"/>
-      <c r="C14" s="67" t="s">
+      <c r="B14" s="89"/>
+      <c r="C14" s="66" t="s">
         <v>168</v>
       </c>
-      <c r="D14" s="71" t="s">
+      <c r="D14" s="70" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3043,14 +3045,14 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="54" t="s">
         <v>149</v>
       </c>
@@ -3064,14 +3066,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="52">
         <v>1</v>
       </c>
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C2" s="76" t="s">
         <v>173</v>
       </c>
       <c r="D2" s="53" t="s">
@@ -3079,59 +3081,59 @@
       </c>
       <c r="F2" s="44"/>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="46">
         <v>2</v>
       </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="78" t="s">
+      <c r="B3" s="90"/>
+      <c r="C3" s="77" t="s">
         <v>174</v>
       </c>
       <c r="D3" s="47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="46">
         <v>3</v>
       </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="78" t="s">
+      <c r="B4" s="90"/>
+      <c r="C4" s="77" t="s">
         <v>175</v>
       </c>
       <c r="D4" s="47" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="46">
         <v>4</v>
       </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="78" t="s">
+      <c r="B5" s="90"/>
+      <c r="C5" s="77" t="s">
         <v>176</v>
       </c>
       <c r="D5" s="47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="46">
         <v>5</v>
       </c>
-      <c r="B6" s="91"/>
-      <c r="C6" s="78" t="s">
+      <c r="B6" s="90"/>
+      <c r="C6" s="77" t="s">
         <v>177</v>
       </c>
       <c r="D6" s="47" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="48">
         <v>6</v>
       </c>
-      <c r="B7" s="90"/>
+      <c r="B7" s="89"/>
       <c r="C7" s="57" t="s">
         <v>178</v>
       </c>
@@ -3139,25 +3141,25 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="45">
         <v>8</v>
       </c>
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="78" t="s">
         <v>179</v>
       </c>
       <c r="D8" s="51" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="48">
         <v>7</v>
       </c>
-      <c r="B9" s="94"/>
+      <c r="B9" s="93"/>
       <c r="C9" s="57" t="s">
         <v>180</v>
       </c>
@@ -3165,7 +3167,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" s="50"/>
       <c r="D11" s="50"/>
     </row>
@@ -3183,18 +3185,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC1D336-9D64-4429-8CDB-FA9C7AC22479}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="58" t="s">
         <v>149</v>
       </c>
@@ -3208,37 +3210,37 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="45">
         <v>1</v>
       </c>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="79" t="s">
         <v>181</v>
       </c>
       <c r="D2" s="61" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="46">
         <v>2</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="78" t="s">
+      <c r="B3" s="95"/>
+      <c r="C3" s="77" t="s">
         <v>217</v>
       </c>
       <c r="D3" s="47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="48">
         <v>3</v>
       </c>
-      <c r="B4" s="97"/>
+      <c r="B4" s="96"/>
       <c r="C4" s="57" t="s">
         <v>218</v>
       </c>
@@ -3246,25 +3248,25 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="45">
         <v>4</v>
       </c>
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="78" t="s">
         <v>182</v>
       </c>
       <c r="D5" s="51" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="48">
         <v>5</v>
       </c>
-      <c r="B6" s="94"/>
+      <c r="B6" s="93"/>
       <c r="C6" s="57" t="s">
         <v>183</v>
       </c>
@@ -3272,29 +3274,29 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="45">
         <v>6</v>
       </c>
-      <c r="B7" s="93" t="s">
+      <c r="B7" s="92" t="s">
         <v>150</v>
       </c>
-      <c r="C7" s="81" t="s">
+      <c r="C7" s="80" t="s">
         <v>184</v>
       </c>
       <c r="D7" s="51" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="48">
         <v>7</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="62" t="s">
+      <c r="B8" s="93"/>
+      <c r="C8" s="97" t="s">
         <v>185</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="62" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>